<commit_message>
added new server and client, working on final
</commit_message>
<xml_diff>
--- a/updated_Burndown.xlsx
+++ b/updated_Burndown.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Source\Kalah_315\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10995"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
   <si>
     <t>PLAN</t>
   </si>
@@ -166,9 +166,6 @@
     <t>6 hr</t>
   </si>
   <si>
-    <t>Kalah Main (updated)</t>
-  </si>
-  <si>
     <t>5 hr</t>
   </si>
   <si>
@@ -186,12 +183,15 @@
   <si>
     <t>Updated Sprint 1 and Sprint 2</t>
   </si>
+  <si>
+    <t>Kalah Main (updated)(scrapped)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -306,6 +306,17 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Corbel"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -473,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -579,7 +590,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -604,20 +614,684 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="198">
+  <dxfs count="233">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6DDB9"/>
+          <bgColor rgb="FFF6DDB9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6DDB9"/>
+          <bgColor rgb="FFF6DDB9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9B8C9"/>
+          <bgColor rgb="FFC9B8C9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9B8C9"/>
+          <bgColor rgb="FFC9B8C9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9AB51"/>
+          <bgColor rgb="FFE9AB51"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9AB51"/>
+          <bgColor rgb="FFE9AB51"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF735773"/>
+          <bgColor rgb="FF735773"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF735773"/>
+          <bgColor rgb="FF735773"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6DDB9"/>
+          <bgColor rgb="FFF6DDB9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6DDB9"/>
+          <bgColor rgb="FFF6DDB9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9B8C9"/>
+          <bgColor rgb="FFC9B8C9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9B8C9"/>
+          <bgColor rgb="FFC9B8C9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9AB51"/>
+          <bgColor rgb="FFE9AB51"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9AB51"/>
+          <bgColor rgb="FFE9AB51"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF735773"/>
+          <bgColor rgb="FF735773"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF735773"/>
+          <bgColor rgb="FF735773"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6DDB9"/>
+          <bgColor rgb="FFF6DDB9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6DDB9"/>
+          <bgColor rgb="FFF6DDB9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9B8C9"/>
+          <bgColor rgb="FFC9B8C9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9B8C9"/>
+          <bgColor rgb="FFC9B8C9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9AB51"/>
+          <bgColor rgb="FFE9AB51"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9AB51"/>
+          <bgColor rgb="FFE9AB51"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF735773"/>
+          <bgColor rgb="FF735773"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF735773"/>
+          <bgColor rgb="FF735773"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -629,115 +1303,6 @@
           <color rgb="FF735773"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6DDB9"/>
-          <bgColor rgb="FFF6DDB9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9B8C9"/>
-          <bgColor rgb="FFC9B8C9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE9AB51"/>
-          <bgColor rgb="FFE9AB51"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF735773"/>
-          <bgColor rgb="FF735773"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3975,49 +4540,46 @@
   <dimension ref="A1:AU72"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AX29" sqref="AX29"/>
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="34.1328125" customWidth="1"/>
-    <col min="3" max="5" width="8.265625" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" customWidth="1"/>
-    <col min="7" max="7" width="8.265625" customWidth="1"/>
-    <col min="8" max="8" width="4.86328125" customWidth="1"/>
-    <col min="9" max="9" width="5.59765625" customWidth="1"/>
-    <col min="10" max="10" width="4.06640625" customWidth="1"/>
-    <col min="11" max="11" width="4.3984375" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" customWidth="1"/>
     <col min="12" max="12" width="4" customWidth="1"/>
-    <col min="13" max="13" width="3.86328125" customWidth="1"/>
-    <col min="14" max="14" width="4.19921875" customWidth="1"/>
-    <col min="15" max="15" width="4.796875" customWidth="1"/>
-    <col min="16" max="18" width="3.1328125" customWidth="1"/>
-    <col min="19" max="19" width="4.3984375" customWidth="1"/>
-    <col min="20" max="20" width="4.46484375" customWidth="1"/>
-    <col min="21" max="21" width="5.3984375" customWidth="1"/>
+    <col min="13" max="13" width="3.85546875" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" customWidth="1"/>
+    <col min="16" max="18" width="3.140625" customWidth="1"/>
+    <col min="19" max="20" width="4.42578125" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
-    <col min="23" max="23" width="4.46484375" customWidth="1"/>
-    <col min="24" max="24" width="4.3984375" customWidth="1"/>
-    <col min="25" max="25" width="4.46484375" customWidth="1"/>
-    <col min="26" max="28" width="3.1328125" customWidth="1"/>
+    <col min="23" max="25" width="4.42578125" customWidth="1"/>
+    <col min="26" max="28" width="3.140625" customWidth="1"/>
     <col min="29" max="29" width="5" customWidth="1"/>
-    <col min="30" max="30" width="4.33203125" customWidth="1"/>
-    <col min="31" max="31" width="5.796875" customWidth="1"/>
-    <col min="32" max="32" width="5.46484375" customWidth="1"/>
-    <col min="33" max="33" width="3.86328125" customWidth="1"/>
-    <col min="34" max="34" width="4.46484375" customWidth="1"/>
+    <col min="30" max="30" width="4.28515625" customWidth="1"/>
+    <col min="31" max="31" width="5.85546875" customWidth="1"/>
+    <col min="32" max="32" width="5.42578125" customWidth="1"/>
+    <col min="33" max="33" width="3.85546875" customWidth="1"/>
+    <col min="34" max="34" width="4.42578125" customWidth="1"/>
     <col min="35" max="35" width="4" customWidth="1"/>
-    <col min="36" max="40" width="3.1328125" customWidth="1"/>
-    <col min="41" max="41" width="3.3984375" customWidth="1"/>
-    <col min="42" max="42" width="4.265625" customWidth="1"/>
-    <col min="43" max="45" width="3.1328125" customWidth="1"/>
-    <col min="46" max="46" width="4.3984375" customWidth="1"/>
+    <col min="36" max="40" width="3.140625" customWidth="1"/>
+    <col min="41" max="41" width="3.42578125" customWidth="1"/>
+    <col min="42" max="42" width="4.28515625" customWidth="1"/>
+    <col min="43" max="45" width="3.140625" customWidth="1"/>
+    <col min="46" max="46" width="4.42578125" customWidth="1"/>
     <col min="47" max="47" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -4047,16 +4609,16 @@
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
     </row>
-    <row r="2" spans="1:47" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:47" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -4079,17 +4641,17 @@
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
     </row>
-    <row r="3" spans="1:47" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:47" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="52" t="s">
-        <v>53</v>
+      <c r="I3" s="49" t="s">
+        <v>52</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -4103,7 +4665,7 @@
       </c>
       <c r="R3" s="4"/>
       <c r="T3" s="9"/>
-      <c r="U3" s="44" t="s">
+      <c r="U3" s="43" t="s">
         <v>42</v>
       </c>
       <c r="V3" s="4"/>
@@ -4115,29 +4677,29 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
-      <c r="AC3" s="48" t="s">
+      <c r="AC3" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD3" s="44" t="s">
         <v>49</v>
-      </c>
-      <c r="AD3" s="45" t="s">
-        <v>50</v>
       </c>
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
       <c r="AI3" s="4"/>
       <c r="AJ3" s="12"/>
-      <c r="AK3" s="45" t="s">
-        <v>51</v>
+      <c r="AK3" s="44" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -4161,7 +4723,7 @@
       <c r="AB4" s="4"/>
       <c r="AS4" s="4"/>
     </row>
-    <row r="5" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -4181,9 +4743,9 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="45" t="s">
-        <v>52</v>
+      <c r="T5" s="48"/>
+      <c r="U5" s="44" t="s">
+        <v>51</v>
       </c>
       <c r="V5" s="22"/>
       <c r="W5" s="22"/>
@@ -4194,7 +4756,7 @@
       <c r="AB5" s="4"/>
       <c r="AS5" s="4"/>
     </row>
-    <row r="6" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
@@ -4235,7 +4797,7 @@
       <c r="AB6" s="4"/>
       <c r="AS6" s="4"/>
     </row>
-    <row r="7" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="14" t="s">
         <v>5</v>
@@ -4300,7 +4862,7 @@
       <c r="AT7" s="22"/>
       <c r="AU7" s="22"/>
     </row>
-    <row r="8" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4321,19 +4883,19 @@
       <c r="L8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="43" t="s">
+      <c r="M8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="43" t="s">
+      <c r="N8" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="43" t="s">
+      <c r="O8" s="42" t="s">
         <v>40</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="18"/>
-      <c r="S8" s="43" t="s">
+      <c r="S8" s="42" t="s">
         <v>34</v>
       </c>
       <c r="T8" s="17" t="s">
@@ -4345,10 +4907,10 @@
       <c r="V8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="W8" s="43" t="s">
+      <c r="W8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="X8" s="43" t="s">
+      <c r="X8" s="42" t="s">
         <v>39</v>
       </c>
       <c r="Y8" s="17" t="s">
@@ -4405,7 +4967,7 @@
       <c r="AT8" s="18"/>
       <c r="AU8" s="20"/>
     </row>
-    <row r="9" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="24" t="s">
         <v>15</v>
@@ -4422,7 +4984,7 @@
       <c r="F9" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="42">
+      <c r="G9" s="41">
         <v>1</v>
       </c>
       <c r="H9" s="35"/>
@@ -4430,8 +4992,8 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="46" t="s">
-        <v>49</v>
+      <c r="M9" s="45" t="s">
+        <v>48</v>
       </c>
       <c r="N9" s="35"/>
       <c r="O9" s="35"/>
@@ -4468,7 +5030,7 @@
       <c r="AT9" s="28"/>
       <c r="AU9" s="26"/>
     </row>
-    <row r="10" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
         <v>14</v>
@@ -4485,7 +5047,7 @@
       <c r="F10" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="41">
         <v>1</v>
       </c>
       <c r="H10" s="35"/>
@@ -4494,8 +5056,8 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="46" t="s">
-        <v>49</v>
+      <c r="N10" s="45" t="s">
+        <v>48</v>
       </c>
       <c r="O10" s="35"/>
       <c r="P10" s="29"/>
@@ -4531,7 +5093,7 @@
       <c r="AT10" s="28"/>
       <c r="AU10" s="26"/>
     </row>
-    <row r="11" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="23" t="s">
         <v>13</v>
@@ -4548,7 +5110,7 @@
       <c r="F11" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="42">
+      <c r="G11" s="41">
         <v>1</v>
       </c>
       <c r="H11" s="35"/>
@@ -4592,7 +5154,7 @@
       <c r="AT11" s="28"/>
       <c r="AU11" s="26"/>
     </row>
-    <row r="12" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="23" t="s">
         <v>16</v>
@@ -4609,7 +5171,7 @@
       <c r="F12" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="41">
         <v>0.95</v>
       </c>
       <c r="H12" s="35"/>
@@ -4619,13 +5181,13 @@
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="49"/>
+      <c r="O12" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="10"/>
       <c r="T12" s="26"/>
       <c r="U12" s="28"/>
       <c r="V12" s="26"/>
@@ -4655,10 +5217,10 @@
       <c r="AT12" s="28"/>
       <c r="AU12" s="26"/>
     </row>
-    <row r="13" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>31</v>
@@ -4670,9 +5232,9 @@
         <v>31</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="42">
+        <v>47</v>
+      </c>
+      <c r="G13" s="41">
         <v>0.85</v>
       </c>
       <c r="H13" s="35"/>
@@ -4683,10 +5245,10 @@
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="49"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="10"/>
       <c r="T13" s="35"/>
       <c r="U13" s="35"/>
       <c r="V13" s="33"/>
@@ -4716,7 +5278,7 @@
       <c r="AT13" s="28"/>
       <c r="AU13" s="26"/>
     </row>
-    <row r="14" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="23" t="s">
         <v>17</v>
@@ -4725,7 +5287,7 @@
       <c r="D14" s="23"/>
       <c r="E14" s="37"/>
       <c r="F14" s="23"/>
-      <c r="G14" s="42"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
       <c r="J14" s="35"/>
@@ -4767,7 +5329,7 @@
       <c r="AT14" s="28"/>
       <c r="AU14" s="26"/>
     </row>
-    <row r="15" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="40" t="s">
         <v>24</v>
@@ -4782,7 +5344,7 @@
         <v>32</v>
       </c>
       <c r="F15" s="23"/>
-      <c r="G15" s="42">
+      <c r="G15" s="41">
         <v>0</v>
       </c>
       <c r="H15" s="35"/>
@@ -4799,12 +5361,14 @@
       <c r="S15" s="35"/>
       <c r="T15" s="35"/>
       <c r="U15" s="35"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="49"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="X15" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y15" s="26"/>
       <c r="Z15" s="28"/>
       <c r="AA15" s="26"/>
       <c r="AB15" s="28"/>
@@ -4828,7 +5392,7 @@
       <c r="AT15" s="30"/>
       <c r="AU15" s="31"/>
     </row>
-    <row r="16" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="40" t="s">
         <v>23</v>
@@ -4843,7 +5407,7 @@
         <v>32</v>
       </c>
       <c r="F16" s="23"/>
-      <c r="G16" s="42">
+      <c r="G16" s="41">
         <v>0</v>
       </c>
       <c r="H16" s="35"/>
@@ -4859,10 +5423,10 @@
       <c r="R16" s="35"/>
       <c r="S16" s="35"/>
       <c r="T16" s="35"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="49"/>
-      <c r="X16" s="25"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="10"/>
       <c r="Y16" s="25"/>
       <c r="Z16" s="25"/>
       <c r="AA16" s="34"/>
@@ -4887,7 +5451,7 @@
       <c r="AT16" s="32"/>
       <c r="AU16" s="32"/>
     </row>
-    <row r="17" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="40" t="s">
         <v>25</v>
@@ -4902,7 +5466,7 @@
         <v>32</v>
       </c>
       <c r="F17" s="23"/>
-      <c r="G17" s="42">
+      <c r="G17" s="41">
         <v>0</v>
       </c>
       <c r="H17" s="35"/>
@@ -4916,13 +5480,13 @@
       <c r="P17" s="35"/>
       <c r="Q17" s="35"/>
       <c r="R17" s="35"/>
-      <c r="S17" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="T17" s="12"/>
-      <c r="U17" s="49"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
+      <c r="S17" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="10"/>
       <c r="X17" s="30"/>
       <c r="Y17" s="31"/>
       <c r="Z17" s="30"/>
@@ -4948,15 +5512,22 @@
       <c r="AT17" s="32"/>
       <c r="AU17" s="32"/>
     </row>
-    <row r="18" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="23"/>
-      <c r="E18" s="23"/>
+        <v>20</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>32</v>
+      </c>
       <c r="F18" s="23"/>
-      <c r="G18" s="42">
+      <c r="G18" s="41">
         <v>0</v>
       </c>
       <c r="H18" s="35"/>
@@ -4974,19 +5545,19 @@
       <c r="T18" s="35"/>
       <c r="U18" s="35"/>
       <c r="V18" s="33"/>
-      <c r="W18" s="33"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="32"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="32"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="33"/>
+      <c r="AB18" s="33"/>
       <c r="AC18" s="33"/>
       <c r="AD18" s="33"/>
       <c r="AE18" s="33"/>
-      <c r="AF18" s="28"/>
-      <c r="AG18" s="26"/>
-      <c r="AH18" s="28"/>
-      <c r="AI18" s="26"/>
+      <c r="AF18" s="33"/>
+      <c r="AG18" s="33"/>
+      <c r="AH18" s="33"/>
+      <c r="AI18" s="33"/>
       <c r="AJ18" s="28"/>
       <c r="AK18" s="26"/>
       <c r="AL18" s="32"/>
@@ -5000,22 +5571,17 @@
       <c r="AT18" s="28"/>
       <c r="AU18" s="26"/>
     </row>
-    <row r="19" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="E19" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="37" t="s">
-        <v>32</v>
-      </c>
       <c r="F19" s="23"/>
-      <c r="G19" s="42">
+      <c r="G19" s="41">
         <v>0</v>
       </c>
       <c r="H19" s="35"/>
@@ -5033,11 +5599,9 @@
       <c r="T19" s="35"/>
       <c r="U19" s="35"/>
       <c r="V19" s="33"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y19" s="49"/>
+      <c r="W19" s="33"/>
+      <c r="X19" s="33"/>
+      <c r="Y19" s="33"/>
       <c r="Z19" s="33"/>
       <c r="AA19" s="33"/>
       <c r="AB19" s="33"/>
@@ -5061,7 +5625,7 @@
       <c r="AT19" s="33"/>
       <c r="AU19" s="33"/>
     </row>
-    <row r="20" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="40" t="s">
         <v>26</v>
@@ -5074,7 +5638,7 @@
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="42">
+      <c r="G20" s="41">
         <v>0</v>
       </c>
       <c r="H20" s="35"/>
@@ -5097,9 +5661,11 @@
       <c r="Y20" s="33"/>
       <c r="Z20" s="33"/>
       <c r="AA20" s="33"/>
-      <c r="AB20" s="33"/>
-      <c r="AC20" s="33"/>
-      <c r="AD20" s="33"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="12"/>
+      <c r="AD20" s="52" t="s">
+        <v>48</v>
+      </c>
       <c r="AE20" s="33"/>
       <c r="AF20" s="33"/>
       <c r="AG20" s="33"/>
@@ -5118,7 +5684,7 @@
       <c r="AT20" s="33"/>
       <c r="AU20" s="33"/>
     </row>
-    <row r="21" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="35" t="s">
         <v>27</v>
@@ -5131,7 +5697,7 @@
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="42">
+      <c r="G21" s="41">
         <v>0</v>
       </c>
       <c r="H21" s="35"/>
@@ -5155,10 +5721,12 @@
       <c r="Z21" s="33"/>
       <c r="AA21" s="33"/>
       <c r="AB21" s="33"/>
-      <c r="AC21" s="33"/>
-      <c r="AD21" s="33"/>
-      <c r="AE21" s="33"/>
-      <c r="AF21" s="33"/>
+      <c r="AC21" s="32"/>
+      <c r="AD21" s="12"/>
+      <c r="AE21" s="12"/>
+      <c r="AF21" s="52" t="s">
+        <v>48</v>
+      </c>
       <c r="AG21" s="33"/>
       <c r="AH21" s="33"/>
       <c r="AI21" s="33"/>
@@ -5175,7 +5743,7 @@
       <c r="AT21" s="33"/>
       <c r="AU21" s="33"/>
     </row>
-    <row r="22" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="35" t="s">
         <v>28</v>
@@ -5188,7 +5756,7 @@
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="42">
+      <c r="G22" s="41">
         <v>0</v>
       </c>
       <c r="H22" s="35"/>
@@ -5215,10 +5783,12 @@
       <c r="AC22" s="33"/>
       <c r="AD22" s="33"/>
       <c r="AE22" s="33"/>
-      <c r="AF22" s="33"/>
-      <c r="AG22" s="33"/>
-      <c r="AH22" s="33"/>
-      <c r="AI22" s="33"/>
+      <c r="AF22" s="53"/>
+      <c r="AG22" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH22" s="53"/>
+      <c r="AI22" s="48"/>
       <c r="AJ22" s="33"/>
       <c r="AK22" s="33"/>
       <c r="AL22" s="33"/>
@@ -5232,7 +5802,7 @@
       <c r="AT22" s="33"/>
       <c r="AU22" s="33"/>
     </row>
-    <row r="23" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="35" t="s">
         <v>29</v>
@@ -5245,7 +5815,7 @@
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
-      <c r="G23" s="42">
+      <c r="G23" s="41">
         <v>0</v>
       </c>
       <c r="H23" s="35"/>
@@ -5272,10 +5842,10 @@
       <c r="AC23" s="33"/>
       <c r="AD23" s="33"/>
       <c r="AE23" s="33"/>
-      <c r="AF23" s="33"/>
-      <c r="AG23" s="33"/>
-      <c r="AH23" s="33"/>
-      <c r="AI23" s="33"/>
+      <c r="AF23" s="12"/>
+      <c r="AG23" s="12"/>
+      <c r="AH23" s="53"/>
+      <c r="AI23" s="48"/>
       <c r="AJ23" s="33"/>
       <c r="AK23" s="33"/>
       <c r="AL23" s="33"/>
@@ -5289,14 +5859,8 @@
       <c r="AT23" s="33"/>
       <c r="AU23" s="33"/>
     </row>
-    <row r="24" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
       <c r="H24" s="35"/>
       <c r="I24" s="35"/>
       <c r="J24" s="35"/>
@@ -5338,14 +5902,8 @@
       <c r="AT24" s="33"/>
       <c r="AU24" s="33"/>
     </row>
-    <row r="25" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
       <c r="H25" s="35"/>
       <c r="I25" s="35"/>
       <c r="J25" s="35"/>
@@ -5387,14 +5945,8 @@
       <c r="AT25" s="33"/>
       <c r="AU25" s="33"/>
     </row>
-    <row r="26" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
       <c r="H26" s="35"/>
       <c r="I26" s="35"/>
       <c r="J26" s="35"/>
@@ -5436,14 +5988,8 @@
       <c r="AT26" s="33"/>
       <c r="AU26" s="33"/>
     </row>
-    <row r="27" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
       <c r="H27" s="35"/>
       <c r="I27" s="35"/>
       <c r="J27" s="35"/>
@@ -5485,7 +6031,7 @@
       <c r="AT27" s="33"/>
       <c r="AU27" s="33"/>
     </row>
-    <row r="28" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="35"/>
       <c r="C28" s="23"/>
@@ -5534,7 +6080,7 @@
       <c r="AT28" s="33"/>
       <c r="AU28" s="33"/>
     </row>
-    <row r="29" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="35"/>
       <c r="C29" s="23"/>
@@ -5583,9 +6129,9 @@
       <c r="AT29" s="33"/>
       <c r="AU29" s="33"/>
     </row>
-    <row r="30" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="35"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
@@ -5632,9 +6178,9 @@
       <c r="AT30" s="33"/>
       <c r="AU30" s="33"/>
     </row>
-    <row r="31" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="23"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
@@ -5681,7 +6227,7 @@
       <c r="AT31" s="33"/>
       <c r="AU31" s="33"/>
     </row>
-    <row r="32" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="35"/>
       <c r="C32" s="23"/>
@@ -5730,7 +6276,7 @@
       <c r="AT32" s="33"/>
       <c r="AU32" s="33"/>
     </row>
-    <row r="33" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="35"/>
       <c r="C33" s="23"/>
@@ -5779,7 +6325,7 @@
       <c r="AT33" s="33"/>
       <c r="AU33" s="33"/>
     </row>
-    <row r="34" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="35"/>
       <c r="C34" s="23"/>
@@ -5828,7 +6374,7 @@
       <c r="AT34" s="33"/>
       <c r="AU34" s="33"/>
     </row>
-    <row r="35" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="35"/>
       <c r="C35" s="23"/>
@@ -5877,7 +6423,7 @@
       <c r="AT35" s="33"/>
       <c r="AU35" s="33"/>
     </row>
-    <row r="36" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="35"/>
       <c r="C36" s="23"/>
@@ -5926,7 +6472,7 @@
       <c r="AT36" s="33"/>
       <c r="AU36" s="33"/>
     </row>
-    <row r="37" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="35"/>
       <c r="C37" s="23"/>
@@ -5975,7 +6521,7 @@
       <c r="AT37" s="33"/>
       <c r="AU37" s="33"/>
     </row>
-    <row r="38" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="35"/>
       <c r="C38" s="23"/>
@@ -6024,7 +6570,7 @@
       <c r="AT38" s="33"/>
       <c r="AU38" s="33"/>
     </row>
-    <row r="39" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="35"/>
       <c r="C39" s="23"/>
@@ -6073,7 +6619,7 @@
       <c r="AT39" s="33"/>
       <c r="AU39" s="33"/>
     </row>
-    <row r="40" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="35"/>
       <c r="C40" s="23"/>
@@ -6122,7 +6668,7 @@
       <c r="AT40" s="33"/>
       <c r="AU40" s="33"/>
     </row>
-    <row r="41" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="35"/>
       <c r="C41" s="23"/>
@@ -6171,7 +6717,7 @@
       <c r="AT41" s="33"/>
       <c r="AU41" s="33"/>
     </row>
-    <row r="42" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="35"/>
       <c r="C42" s="23"/>
@@ -6220,7 +6766,7 @@
       <c r="AT42" s="33"/>
       <c r="AU42" s="33"/>
     </row>
-    <row r="43" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="35"/>
       <c r="C43" s="23"/>
@@ -6269,7 +6815,7 @@
       <c r="AT43" s="33"/>
       <c r="AU43" s="33"/>
     </row>
-    <row r="44" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="35"/>
       <c r="C44" s="23"/>
@@ -6318,7 +6864,7 @@
       <c r="AT44" s="33"/>
       <c r="AU44" s="33"/>
     </row>
-    <row r="45" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="35"/>
       <c r="C45" s="23"/>
@@ -6367,7 +6913,7 @@
       <c r="AT45" s="33"/>
       <c r="AU45" s="33"/>
     </row>
-    <row r="46" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="35"/>
       <c r="C46" s="23"/>
@@ -6416,7 +6962,7 @@
       <c r="AT46" s="33"/>
       <c r="AU46" s="33"/>
     </row>
-    <row r="47" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="35"/>
       <c r="C47" s="23"/>
@@ -6465,7 +7011,7 @@
       <c r="AT47" s="33"/>
       <c r="AU47" s="33"/>
     </row>
-    <row r="48" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="35"/>
       <c r="C48" s="23"/>
@@ -6514,14 +7060,14 @@
       <c r="AT48" s="33"/>
       <c r="AU48" s="33"/>
     </row>
-    <row r="49" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="35"/>
       <c r="C49" s="23"/>
       <c r="D49" s="23"/>
       <c r="E49" s="23"/>
       <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
+      <c r="G49" s="39"/>
       <c r="H49" s="35"/>
       <c r="I49" s="35"/>
       <c r="J49" s="35"/>
@@ -6563,7 +7109,7 @@
       <c r="AT49" s="33"/>
       <c r="AU49" s="33"/>
     </row>
-    <row r="50" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="35"/>
       <c r="C50" s="23"/>
@@ -6612,7 +7158,7 @@
       <c r="AT50" s="33"/>
       <c r="AU50" s="33"/>
     </row>
-    <row r="51" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="35"/>
       <c r="C51" s="23"/>
@@ -6661,7 +7207,7 @@
       <c r="AT51" s="33"/>
       <c r="AU51" s="33"/>
     </row>
-    <row r="52" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="35"/>
       <c r="C52" s="23"/>
@@ -6710,22 +7256,22 @@
       <c r="AT52" s="33"/>
       <c r="AU52" s="33"/>
     </row>
-    <row r="53" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="35"/>
-      <c r="O53" s="35"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+      <c r="N53" s="33"/>
+      <c r="O53" s="33"/>
       <c r="P53" s="35"/>
       <c r="Q53" s="35"/>
       <c r="R53" s="35"/>
@@ -6759,7 +7305,7 @@
       <c r="AT53" s="33"/>
       <c r="AU53" s="33"/>
     </row>
-    <row r="54" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="36"/>
       <c r="C54" s="35"/>
@@ -6781,8 +7327,8 @@
       <c r="S54" s="35"/>
       <c r="T54" s="35"/>
       <c r="U54" s="35"/>
-      <c r="V54" s="33"/>
-      <c r="W54" s="33"/>
+      <c r="V54" s="35"/>
+      <c r="W54" s="35"/>
       <c r="X54" s="33"/>
       <c r="Y54" s="33"/>
       <c r="Z54" s="33"/>
@@ -6808,7 +7354,7 @@
       <c r="AT54" s="33"/>
       <c r="AU54" s="33"/>
     </row>
-    <row r="55" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="36"/>
       <c r="C55" s="35"/>
@@ -6857,7 +7403,7 @@
       <c r="AT55" s="33"/>
       <c r="AU55" s="33"/>
     </row>
-    <row r="56" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="36"/>
       <c r="C56" s="35"/>
@@ -6906,42 +7452,13 @@
       <c r="AT56" s="33"/>
       <c r="AU56" s="33"/>
     </row>
-    <row r="57" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="33"/>
-      <c r="O57" s="33"/>
-      <c r="P57" s="35"/>
-      <c r="Q57" s="35"/>
-      <c r="R57" s="35"/>
-      <c r="S57" s="35"/>
-      <c r="T57" s="35"/>
-      <c r="U57" s="35"/>
-      <c r="V57" s="35"/>
-      <c r="W57" s="35"/>
-      <c r="X57" s="33"/>
-      <c r="Y57" s="33"/>
-      <c r="Z57" s="33"/>
-      <c r="AA57" s="33"/>
-      <c r="AB57" s="33"/>
-      <c r="AC57" s="33"/>
-      <c r="AD57" s="33"/>
-      <c r="AE57" s="33"/>
-      <c r="AF57" s="33"/>
-      <c r="AG57" s="33"/>
-      <c r="AH57" s="33"/>
-      <c r="AI57" s="33"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
       <c r="AJ57" s="33"/>
       <c r="AK57" s="33"/>
       <c r="AL57" s="33"/>
@@ -6955,13 +7472,8 @@
       <c r="AT57" s="33"/>
       <c r="AU57" s="33"/>
     </row>
-    <row r="58" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="4"/>
-      <c r="V58" s="4"/>
-      <c r="W58" s="4"/>
       <c r="AL58" s="22"/>
       <c r="AM58" s="22"/>
       <c r="AN58" s="22"/>
@@ -6973,7 +7485,7 @@
       <c r="AT58" s="22"/>
       <c r="AU58" s="22"/>
     </row>
-    <row r="59" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="AL59" s="22"/>
       <c r="AM59" s="22"/>
@@ -6986,7 +7498,7 @@
       <c r="AT59" s="22"/>
       <c r="AU59" s="22"/>
     </row>
-    <row r="60" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="AL60" s="22"/>
       <c r="AM60" s="22"/>
@@ -6999,1034 +7511,1104 @@
       <c r="AT60" s="22"/>
       <c r="AU60" s="22"/>
     </row>
-    <row r="61" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="P8:R8 I50:O53 Z8:AB8 AJ8:AK8 AC61:AL65 X25:AB65 S14:W14 B22:D22 B18:C18 D15:D17 B21:C21 B25:D53 H13 E12:H12 P14:R57 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 S18:W18 T16 S24:W58 V24:AB24 T23:V23 AB23 U15 V9:AB14 V17:AB18 X16:AB16 Z15:AB15 E25:O49 B14:O14 H19:O24 D23 D19:D21 E20:G23 S20:AB22 S19:V19 Z19:AB19 E18:O18 F15:O17 F19:G19 AC9:AK60">
-    <cfRule type="expression" dxfId="197" priority="227">
+  <conditionalFormatting sqref="P8:R8 I49:O52 Z8:AB8 AJ8:AK8 S14:W14 B22:D22 B19:C19 B21:C21 B28:D52 H13 E12:H12 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 T16 S23:W57 T22:V22 U15 V9:AB14 X17:AB17 Y16:AB16 Z15:AB15 E28:O48 B14:O14 D23 S19:AB19 S18:V18 AA18:AB18 F15:O17 F18:G18 AC9:AK17 D15:D18 D20:D21 E19:G23 AJ61:AL65 P14:R56 AJ18:AK60 AC18:AI19 H18:O27 X24:AI64 AE20:AI20 S21:AB21 S20:AA20 AG21:AI21 AB22:AD22 V23:AE23">
+    <cfRule type="expression" dxfId="232" priority="248">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:R8 I50:O53 Z8:AB8 AJ8:AK8 AC61:AL65 X25:AB65 S14:W14 B22:D22 B18:C18 D15:D17 B21:C21 B25:D53 H13 E12:H12 P14:R57 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 S18:W18 T16 S24:W58 V24:AB24 T23:V23 AB23 U15 V9:AB14 V17:AB18 X16:AB16 Z15:AB15 E25:O49 B14:O14 H19:O24 D23 D19:D21 E20:G23 S20:AB22 S19:V19 Z19:AB19 E18:O18 F15:O17 F19:G19 AC9:AK60">
-    <cfRule type="expression" dxfId="196" priority="228">
+  <conditionalFormatting sqref="P8:R8 I49:O52 Z8:AB8 AJ8:AK8 S14:W14 B22:D22 B19:C19 B21:C21 B28:D52 H13 E12:H12 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 T16 S23:W57 T22:V22 U15 V9:AB14 X17:AB17 Y16:AB16 Z15:AB15 E28:O48 B14:O14 D23 S19:AB19 S18:V18 AA18:AB18 F15:O17 F18:G18 AC9:AK17 D15:D18 D20:D21 E19:G23 AJ61:AL65 P14:R56 AJ18:AK60 AC18:AI19 H18:O27 X24:AI64 AE20:AI20 S21:AB21 S20:AA20 AG21:AI21 AB22:AD22 V23:AE23">
+    <cfRule type="expression" dxfId="231" priority="249">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:R8 I50:O53 Z8:AB8 AJ8:AK8 AC61:AL65 X25:AB65 S14:W14 B22:D22 B18:C18 D15:D17 B21:C21 B25:D53 H13 E12:H12 P14:R57 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 S18:W18 T16 S24:W58 V24:AB24 T23:V23 AB23 U15 V9:AB14 V17:AB18 X16:AB16 Z15:AB15 E25:O49 B14:O14 H19:O24 D23 D19:D21 E20:G23 S20:AB22 S19:V19 Z19:AB19 E18:O18 F15:O17 F19:G19 AC9:AK60">
-    <cfRule type="expression" dxfId="195" priority="229">
+  <conditionalFormatting sqref="P8:R8 I49:O52 Z8:AB8 AJ8:AK8 S14:W14 B22:D22 B19:C19 B21:C21 B28:D52 H13 E12:H12 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 T16 S23:W57 T22:V22 U15 V9:AB14 X17:AB17 Y16:AB16 Z15:AB15 E28:O48 B14:O14 D23 S19:AB19 S18:V18 AA18:AB18 F15:O17 F18:G18 AC9:AK17 D15:D18 D20:D21 E19:G23 AJ61:AL65 P14:R56 AJ18:AK60 AC18:AI19 H18:O27 X24:AI64 AE20:AI20 S21:AB21 S20:AA20 AG21:AI21 AB22:AD22 V23:AE23">
+    <cfRule type="expression" dxfId="230" priority="250">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:R8 I50:O53 Z8:AB8 AJ8:AK8 AC61:AL65 X25:AB65 S14:W14 B22:D22 B18:C18 D15:D17 B21:C21 B25:D53 H13 E12:H12 P14:R57 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 S18:W18 T16 S24:W58 V24:AB24 T23:V23 AB23 U15 V9:AB14 V17:AB18 X16:AB16 Z15:AB15 E25:O49 B14:O14 H19:O24 D23 D19:D21 E20:G23 S20:AB22 S19:V19 Z19:AB19 E18:O18 F15:O17 F19:G19 AC9:AK60">
-    <cfRule type="expression" dxfId="194" priority="230">
+  <conditionalFormatting sqref="P8:R8 I49:O52 Z8:AB8 AJ8:AK8 S14:W14 B22:D22 B19:C19 B21:C21 B28:D52 H13 E12:H12 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 T16 S23:W57 T22:V22 U15 V9:AB14 X17:AB17 Y16:AB16 Z15:AB15 E28:O48 B14:O14 D23 S19:AB19 S18:V18 AA18:AB18 F15:O17 F18:G18 AC9:AK17 D15:D18 D20:D21 E19:G23 AJ61:AL65 P14:R56 AJ18:AK60 AC18:AI19 H18:O27 X24:AI64 AE20:AI20 S21:AB21 S20:AA20 AG21:AI21 AB22:AD22 V23:AE23">
+    <cfRule type="expression" dxfId="229" priority="251">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:R8 I50:O53 Z8:AB8 AJ8:AK8 AC61:AL65 X25:AB65 S14:W14 B22:D22 B18:C18 D15:D17 B21:C21 B25:D53 H13 E12:H12 P14:R57 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 S18:W18 T16 S24:W58 V24:AB24 T23:V23 AB23 U15 V9:AB14 V17:AB18 X16:AB16 Z15:AB15 E25:O49 B14:O14 H19:O24 D23 D19:D21 E20:G23 S20:AB22 S19:V19 Z19:AB19 E18:O18 F15:O17 F19:G19 AC9:AK60">
-    <cfRule type="expression" dxfId="193" priority="231">
+  <conditionalFormatting sqref="P8:R8 I49:O52 Z8:AB8 AJ8:AK8 S14:W14 B22:D22 B19:C19 B21:C21 B28:D52 H13 E12:H12 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 T16 S23:W57 T22:V22 U15 V9:AB14 X17:AB17 Y16:AB16 Z15:AB15 E28:O48 B14:O14 D23 S19:AB19 S18:V18 AA18:AB18 F15:O17 F18:G18 AC9:AK17 D15:D18 D20:D21 E19:G23 AJ61:AL65 P14:R56 AJ18:AK60 AC18:AI19 H18:O27 X24:AI64 AE20:AI20 S21:AB21 S20:AA20 AG21:AI21 AB22:AD22 V23:AE23">
+    <cfRule type="expression" dxfId="228" priority="252">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:R8 I50:O53 Z8:AB8 AJ8:AK8 AC61:AL65 X25:AB65 S14:W14 B22:D22 B18:C18 D15:D17 B21:C21 B25:D53 H13 E12:H12 P14:R57 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 S18:W18 T16 S24:W58 V24:AB24 T23:V23 AB23 U15 V9:AB14 V17:AB18 X16:AB16 Z15:AB15 E25:O49 B14:O14 H19:O24 D23 D19:D21 E20:G23 S20:AB22 S19:V19 Z19:AB19 E18:O18 F15:O17 F19:G19 AC9:AK60">
-    <cfRule type="expression" dxfId="192" priority="232">
+  <conditionalFormatting sqref="P8:R8 I49:O52 Z8:AB8 AJ8:AK8 S14:W14 B22:D22 B19:C19 B21:C21 B28:D52 H13 E12:H12 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 T16 S23:W57 T22:V22 U15 V9:AB14 X17:AB17 Y16:AB16 Z15:AB15 E28:O48 B14:O14 D23 S19:AB19 S18:V18 AA18:AB18 F15:O17 F18:G18 AC9:AK17 D15:D18 D20:D21 E19:G23 AJ61:AL65 P14:R56 AJ18:AK60 AC18:AI19 H18:O27 X24:AI64 AE20:AI20 S21:AB21 S20:AA20 AG21:AI21 AB22:AD22 V23:AE23">
+    <cfRule type="expression" dxfId="227" priority="253">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:R8 I50:O53 Z8:AB8 AJ8:AK8 AC61:AL65 X25:AB65 S14:W14 B22:D22 B18:C18 D15:D17 B21:C21 B25:D53 H13 E12:H12 P14:R57 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 S18:W18 T16 S24:W58 V24:AB24 T23:V23 AB23 U15 V9:AB14 V17:AB18 X16:AB16 Z15:AB15 E25:O49 B14:O14 H19:O24 D23 D19:D21 E20:G23 S20:AB22 S19:V19 Z19:AB19 E18:O18 F15:O17 F19:G19 AC9:AK60">
-    <cfRule type="expression" dxfId="191" priority="233">
+  <conditionalFormatting sqref="P8:R8 I49:O52 Z8:AB8 AJ8:AK8 S14:W14 B22:D22 B19:C19 B21:C21 B28:D52 H13 E12:H12 O10:U10 N9:U9 B9:H11 M11:U11 T12:U12 T13:W13 T16 S23:W57 T22:V22 U15 V9:AB14 X17:AB17 Y16:AB16 Z15:AB15 E28:O48 B14:O14 D23 S19:AB19 S18:V18 AA18:AB18 F15:O17 F18:G18 AC9:AK17 D15:D18 D20:D21 E19:G23 AJ61:AL65 P14:R56 AJ18:AK60 AC18:AI19 H18:O27 X24:AI64 AE20:AI20 S21:AB21 S20:AA20 AG21:AI21 AB22:AD22 V23:AE23">
+    <cfRule type="expression" dxfId="226" priority="254">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18:U18 AC32:AE32 AF33:AK33 P19:R19 L14:O14 X33:AB33 V19 D20 H14 F15:G15">
-    <cfRule type="expression" dxfId="190" priority="234">
+  <conditionalFormatting sqref="AC31:AE31 P18:R18 L14:O14 X32:AB32 V18 D20 H14 F15:G15 AJ33:AK33 AF32:AI32">
+    <cfRule type="expression" dxfId="225" priority="255">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="expression" dxfId="189" priority="213">
+    <cfRule type="expression" dxfId="224" priority="234">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="expression" dxfId="188" priority="214">
+    <cfRule type="expression" dxfId="223" priority="235">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="expression" dxfId="187" priority="215">
+    <cfRule type="expression" dxfId="222" priority="236">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="expression" dxfId="186" priority="216">
+    <cfRule type="expression" dxfId="221" priority="237">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="expression" dxfId="185" priority="217">
+    <cfRule type="expression" dxfId="220" priority="238">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="expression" dxfId="184" priority="218">
+    <cfRule type="expression" dxfId="219" priority="239">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="expression" dxfId="183" priority="219">
+    <cfRule type="expression" dxfId="218" priority="240">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="182" priority="198">
+    <cfRule type="expression" dxfId="217" priority="219">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="181" priority="199">
+    <cfRule type="expression" dxfId="216" priority="220">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="180" priority="200">
+    <cfRule type="expression" dxfId="215" priority="221">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="179" priority="201">
+    <cfRule type="expression" dxfId="214" priority="222">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="178" priority="202">
+    <cfRule type="expression" dxfId="213" priority="223">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="177" priority="203">
+    <cfRule type="expression" dxfId="212" priority="224">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="176" priority="204">
+    <cfRule type="expression" dxfId="211" priority="225">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="175" priority="191">
+    <cfRule type="expression" dxfId="210" priority="212">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="174" priority="192">
+    <cfRule type="expression" dxfId="209" priority="213">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="173" priority="193">
+    <cfRule type="expression" dxfId="208" priority="214">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="172" priority="194">
+    <cfRule type="expression" dxfId="207" priority="215">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="171" priority="195">
+    <cfRule type="expression" dxfId="206" priority="216">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="170" priority="196">
+    <cfRule type="expression" dxfId="205" priority="217">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="169" priority="197">
+    <cfRule type="expression" dxfId="204" priority="218">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="168" priority="184">
+    <cfRule type="expression" dxfId="203" priority="205">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="167" priority="185">
+    <cfRule type="expression" dxfId="202" priority="206">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="166" priority="186">
+    <cfRule type="expression" dxfId="201" priority="207">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="165" priority="187">
+    <cfRule type="expression" dxfId="200" priority="208">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="164" priority="188">
+    <cfRule type="expression" dxfId="199" priority="209">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="163" priority="189">
+    <cfRule type="expression" dxfId="198" priority="210">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="162" priority="190">
+    <cfRule type="expression" dxfId="197" priority="211">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="expression" dxfId="161" priority="177">
+    <cfRule type="expression" dxfId="196" priority="198">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="expression" dxfId="160" priority="178">
+    <cfRule type="expression" dxfId="195" priority="199">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="expression" dxfId="159" priority="179">
+    <cfRule type="expression" dxfId="194" priority="200">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="expression" dxfId="158" priority="180">
+    <cfRule type="expression" dxfId="193" priority="201">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="expression" dxfId="157" priority="181">
+    <cfRule type="expression" dxfId="192" priority="202">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="expression" dxfId="156" priority="182">
+    <cfRule type="expression" dxfId="191" priority="203">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="expression" dxfId="155" priority="183">
+    <cfRule type="expression" dxfId="190" priority="204">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="154" priority="170">
+    <cfRule type="expression" dxfId="189" priority="191">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="153" priority="171">
+    <cfRule type="expression" dxfId="188" priority="192">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="152" priority="172">
+    <cfRule type="expression" dxfId="187" priority="193">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="151" priority="173">
+    <cfRule type="expression" dxfId="186" priority="194">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="150" priority="174">
+    <cfRule type="expression" dxfId="185" priority="195">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="149" priority="175">
+    <cfRule type="expression" dxfId="184" priority="196">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="148" priority="176">
+    <cfRule type="expression" dxfId="183" priority="197">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
-    <cfRule type="expression" dxfId="147" priority="163">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="expression" dxfId="182" priority="184">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
-    <cfRule type="expression" dxfId="146" priority="164">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="expression" dxfId="181" priority="185">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
-    <cfRule type="expression" dxfId="145" priority="165">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="expression" dxfId="180" priority="186">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
-    <cfRule type="expression" dxfId="144" priority="166">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="expression" dxfId="179" priority="187">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
-    <cfRule type="expression" dxfId="143" priority="167">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="expression" dxfId="178" priority="188">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
-    <cfRule type="expression" dxfId="142" priority="168">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="expression" dxfId="177" priority="189">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
-    <cfRule type="expression" dxfId="141" priority="169">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="expression" dxfId="176" priority="190">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="140" priority="156">
+    <cfRule type="expression" dxfId="175" priority="177">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="139" priority="157">
+    <cfRule type="expression" dxfId="174" priority="178">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="138" priority="158">
+    <cfRule type="expression" dxfId="173" priority="179">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="137" priority="159">
+    <cfRule type="expression" dxfId="172" priority="180">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="136" priority="160">
+    <cfRule type="expression" dxfId="171" priority="181">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="135" priority="161">
+    <cfRule type="expression" dxfId="170" priority="182">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="134" priority="162">
+    <cfRule type="expression" dxfId="169" priority="183">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="133" priority="58">
+    <cfRule type="expression" dxfId="168" priority="79">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="132" priority="59">
+    <cfRule type="expression" dxfId="167" priority="80">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="131" priority="60">
+    <cfRule type="expression" dxfId="166" priority="81">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="130" priority="61">
+    <cfRule type="expression" dxfId="165" priority="82">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="129" priority="62">
+    <cfRule type="expression" dxfId="164" priority="83">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="128" priority="63">
+    <cfRule type="expression" dxfId="163" priority="84">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="127" priority="64">
+    <cfRule type="expression" dxfId="162" priority="85">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="126" priority="135">
+    <cfRule type="expression" dxfId="161" priority="156">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="125" priority="136">
+    <cfRule type="expression" dxfId="160" priority="157">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="124" priority="137">
+    <cfRule type="expression" dxfId="159" priority="158">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="123" priority="138">
+    <cfRule type="expression" dxfId="158" priority="159">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="122" priority="139">
+    <cfRule type="expression" dxfId="157" priority="160">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="121" priority="140">
+    <cfRule type="expression" dxfId="156" priority="161">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="120" priority="141">
+    <cfRule type="expression" dxfId="155" priority="162">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="119" priority="128">
+    <cfRule type="expression" dxfId="154" priority="149">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="118" priority="129">
+    <cfRule type="expression" dxfId="153" priority="150">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="117" priority="130">
+    <cfRule type="expression" dxfId="152" priority="151">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="116" priority="131">
+    <cfRule type="expression" dxfId="151" priority="152">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="115" priority="132">
+    <cfRule type="expression" dxfId="150" priority="153">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="114" priority="133">
+    <cfRule type="expression" dxfId="149" priority="154">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="113" priority="134">
+    <cfRule type="expression" dxfId="148" priority="155">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="112" priority="121">
+    <cfRule type="expression" dxfId="147" priority="142">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="111" priority="122">
+    <cfRule type="expression" dxfId="146" priority="143">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="110" priority="123">
+    <cfRule type="expression" dxfId="145" priority="144">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="109" priority="124">
+    <cfRule type="expression" dxfId="144" priority="145">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="108" priority="125">
+    <cfRule type="expression" dxfId="143" priority="146">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="107" priority="126">
+    <cfRule type="expression" dxfId="142" priority="147">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="106" priority="127">
+    <cfRule type="expression" dxfId="141" priority="148">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="105" priority="114">
+    <cfRule type="expression" dxfId="140" priority="135">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="104" priority="115">
+    <cfRule type="expression" dxfId="139" priority="136">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="103" priority="116">
+    <cfRule type="expression" dxfId="138" priority="137">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="102" priority="117">
+    <cfRule type="expression" dxfId="137" priority="138">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="101" priority="118">
+    <cfRule type="expression" dxfId="136" priority="139">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="100" priority="119">
+    <cfRule type="expression" dxfId="135" priority="140">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="99" priority="120">
+    <cfRule type="expression" dxfId="134" priority="141">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="98" priority="79">
+    <cfRule type="expression" dxfId="133" priority="100">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="97" priority="80">
+    <cfRule type="expression" dxfId="132" priority="101">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="96" priority="81">
+    <cfRule type="expression" dxfId="131" priority="102">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="95" priority="82">
+    <cfRule type="expression" dxfId="130" priority="103">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="94" priority="83">
+    <cfRule type="expression" dxfId="129" priority="104">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="93" priority="84">
+    <cfRule type="expression" dxfId="128" priority="105">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="92" priority="85">
+    <cfRule type="expression" dxfId="127" priority="106">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="91" priority="100">
+    <cfRule type="expression" dxfId="126" priority="121">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="90" priority="101">
+    <cfRule type="expression" dxfId="125" priority="122">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="89" priority="102">
+    <cfRule type="expression" dxfId="124" priority="123">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="88" priority="103">
+    <cfRule type="expression" dxfId="123" priority="124">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="87" priority="104">
+    <cfRule type="expression" dxfId="122" priority="125">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="86" priority="105">
+    <cfRule type="expression" dxfId="121" priority="126">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="85" priority="106">
+    <cfRule type="expression" dxfId="120" priority="127">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="84" priority="93">
+    <cfRule type="expression" dxfId="119" priority="114">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="83" priority="94">
+    <cfRule type="expression" dxfId="118" priority="115">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="82" priority="95">
+    <cfRule type="expression" dxfId="117" priority="116">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="81" priority="96">
+    <cfRule type="expression" dxfId="116" priority="117">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="80" priority="97">
+    <cfRule type="expression" dxfId="115" priority="118">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="79" priority="98">
+    <cfRule type="expression" dxfId="114" priority="119">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="78" priority="99">
+    <cfRule type="expression" dxfId="113" priority="120">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="77" priority="86">
+    <cfRule type="expression" dxfId="112" priority="107">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="76" priority="87">
+    <cfRule type="expression" dxfId="111" priority="108">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="75" priority="88">
+    <cfRule type="expression" dxfId="110" priority="109">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="74" priority="89">
+    <cfRule type="expression" dxfId="109" priority="110">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="73" priority="90">
+    <cfRule type="expression" dxfId="108" priority="111">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="72" priority="91">
+    <cfRule type="expression" dxfId="107" priority="112">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="71" priority="92">
+    <cfRule type="expression" dxfId="106" priority="113">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="70" priority="72">
+    <cfRule type="expression" dxfId="105" priority="93">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="69" priority="73">
+    <cfRule type="expression" dxfId="104" priority="94">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="68" priority="74">
+    <cfRule type="expression" dxfId="103" priority="95">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="67" priority="75">
+    <cfRule type="expression" dxfId="102" priority="96">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="66" priority="76">
+    <cfRule type="expression" dxfId="101" priority="97">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="65" priority="77">
+    <cfRule type="expression" dxfId="100" priority="98">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="64" priority="78">
+    <cfRule type="expression" dxfId="99" priority="99">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="63" priority="65">
+  <conditionalFormatting sqref="S22">
+    <cfRule type="expression" dxfId="98" priority="86">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="62" priority="66">
+  <conditionalFormatting sqref="S22">
+    <cfRule type="expression" dxfId="97" priority="87">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="61" priority="67">
+  <conditionalFormatting sqref="S22">
+    <cfRule type="expression" dxfId="96" priority="88">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="60" priority="68">
+  <conditionalFormatting sqref="S22">
+    <cfRule type="expression" dxfId="95" priority="89">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="59" priority="69">
+  <conditionalFormatting sqref="S22">
+    <cfRule type="expression" dxfId="94" priority="90">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="58" priority="70">
+  <conditionalFormatting sqref="S22">
+    <cfRule type="expression" dxfId="93" priority="91">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="expression" dxfId="57" priority="71">
+  <conditionalFormatting sqref="S22">
+    <cfRule type="expression" dxfId="92" priority="92">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16">
-    <cfRule type="expression" dxfId="56" priority="51">
+    <cfRule type="expression" dxfId="91" priority="72">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16">
-    <cfRule type="expression" dxfId="55" priority="52">
+    <cfRule type="expression" dxfId="90" priority="73">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16">
-    <cfRule type="expression" dxfId="54" priority="53">
+    <cfRule type="expression" dxfId="89" priority="74">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16">
-    <cfRule type="expression" dxfId="53" priority="54">
+    <cfRule type="expression" dxfId="88" priority="75">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16">
-    <cfRule type="expression" dxfId="52" priority="55">
+    <cfRule type="expression" dxfId="87" priority="76">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16">
-    <cfRule type="expression" dxfId="51" priority="56">
+    <cfRule type="expression" dxfId="86" priority="77">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16">
-    <cfRule type="expression" dxfId="50" priority="57">
+    <cfRule type="expression" dxfId="85" priority="78">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="49" priority="44">
+    <cfRule type="expression" dxfId="84" priority="65">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="48" priority="45">
+    <cfRule type="expression" dxfId="83" priority="66">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="47" priority="46">
+    <cfRule type="expression" dxfId="82" priority="67">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="46" priority="47">
+    <cfRule type="expression" dxfId="81" priority="68">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="45" priority="48">
+    <cfRule type="expression" dxfId="80" priority="69">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="44" priority="49">
+    <cfRule type="expression" dxfId="79" priority="70">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="43" priority="50">
+    <cfRule type="expression" dxfId="78" priority="71">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:G24">
-    <cfRule type="expression" dxfId="42" priority="37">
+  <conditionalFormatting sqref="Z22:AA22">
+    <cfRule type="expression" dxfId="77" priority="51">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:G24">
-    <cfRule type="expression" dxfId="41" priority="38">
+  <conditionalFormatting sqref="Z22:AA22">
+    <cfRule type="expression" dxfId="76" priority="52">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:G24">
-    <cfRule type="expression" dxfId="40" priority="39">
+  <conditionalFormatting sqref="Z22:AA22">
+    <cfRule type="expression" dxfId="75" priority="53">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:G24">
-    <cfRule type="expression" dxfId="39" priority="40">
+  <conditionalFormatting sqref="Z22:AA22">
+    <cfRule type="expression" dxfId="74" priority="54">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:G24">
-    <cfRule type="expression" dxfId="38" priority="41">
+  <conditionalFormatting sqref="Z22:AA22">
+    <cfRule type="expression" dxfId="73" priority="55">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:G24">
-    <cfRule type="expression" dxfId="37" priority="42">
+  <conditionalFormatting sqref="Z22:AA22">
+    <cfRule type="expression" dxfId="72" priority="56">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:G24">
-    <cfRule type="expression" dxfId="36" priority="43">
+  <conditionalFormatting sqref="Z22:AA22">
+    <cfRule type="expression" dxfId="71" priority="57">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z23:AA23">
-    <cfRule type="expression" dxfId="35" priority="30">
+  <conditionalFormatting sqref="W22:Y22">
+    <cfRule type="expression" dxfId="70" priority="44">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z23:AA23">
-    <cfRule type="expression" dxfId="34" priority="31">
+  <conditionalFormatting sqref="W22:Y22">
+    <cfRule type="expression" dxfId="69" priority="45">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z23:AA23">
-    <cfRule type="expression" dxfId="33" priority="32">
+  <conditionalFormatting sqref="W22:Y22">
+    <cfRule type="expression" dxfId="68" priority="46">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z23:AA23">
-    <cfRule type="expression" dxfId="32" priority="33">
+  <conditionalFormatting sqref="W22:Y22">
+    <cfRule type="expression" dxfId="67" priority="47">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z23:AA23">
-    <cfRule type="expression" dxfId="31" priority="34">
+  <conditionalFormatting sqref="W22:Y22">
+    <cfRule type="expression" dxfId="66" priority="48">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z23:AA23">
-    <cfRule type="expression" dxfId="30" priority="35">
+  <conditionalFormatting sqref="W22:Y22">
+    <cfRule type="expression" dxfId="65" priority="49">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z23:AA23">
-    <cfRule type="expression" dxfId="29" priority="36">
+  <conditionalFormatting sqref="W22:Y22">
+    <cfRule type="expression" dxfId="64" priority="50">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W23:Y23">
-    <cfRule type="expression" dxfId="28" priority="23">
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="expression" dxfId="63" priority="37">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W23:Y23">
-    <cfRule type="expression" dxfId="27" priority="24">
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="expression" dxfId="62" priority="38">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W23:Y23">
-    <cfRule type="expression" dxfId="26" priority="25">
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="expression" dxfId="61" priority="39">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W23:Y23">
-    <cfRule type="expression" dxfId="25" priority="26">
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="expression" dxfId="60" priority="40">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W23:Y23">
-    <cfRule type="expression" dxfId="24" priority="27">
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="expression" dxfId="59" priority="41">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W23:Y23">
-    <cfRule type="expression" dxfId="23" priority="28">
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="expression" dxfId="58" priority="42">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W23:Y23">
-    <cfRule type="expression" dxfId="22" priority="29">
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="expression" dxfId="57" priority="43">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="21" priority="16">
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="56" priority="30">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="20" priority="17">
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="55" priority="31">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="19" priority="18">
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="54" priority="32">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="18" priority="19">
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="53" priority="33">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="17" priority="20">
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="52" priority="34">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="16" priority="21">
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="51" priority="35">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="15" priority="22">
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="50" priority="36">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="14" priority="9">
+  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
+    <cfRule type="expression" dxfId="49" priority="22">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="13" priority="10">
+  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
+    <cfRule type="expression" dxfId="48" priority="23">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="12" priority="11">
+  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
+    <cfRule type="expression" dxfId="47" priority="24">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="11" priority="12">
+  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
+    <cfRule type="expression" dxfId="46" priority="25">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="10" priority="13">
+  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
+    <cfRule type="expression" dxfId="45" priority="26">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="9" priority="14">
+  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
+    <cfRule type="expression" dxfId="44" priority="27">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="8" priority="15">
+  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
+    <cfRule type="expression" dxfId="43" priority="28">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="AM32:AO32 AP33:AU33 AL33">
+    <cfRule type="expression" dxfId="42" priority="29">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE22">
+    <cfRule type="expression" dxfId="41" priority="15">
       <formula>PercentComplete</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
-    <cfRule type="expression" dxfId="6" priority="2">
+  <conditionalFormatting sqref="AE22">
+    <cfRule type="expression" dxfId="39" priority="16">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
-    <cfRule type="expression" dxfId="5" priority="3">
+  <conditionalFormatting sqref="AE22">
+    <cfRule type="expression" dxfId="37" priority="17">
       <formula>Actual</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
-    <cfRule type="expression" dxfId="4" priority="4">
+  <conditionalFormatting sqref="AE22">
+    <cfRule type="expression" dxfId="35" priority="18">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
-    <cfRule type="expression" dxfId="3" priority="5">
+  <conditionalFormatting sqref="AE22">
+    <cfRule type="expression" dxfId="33" priority="19">
       <formula>Plan</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
-    <cfRule type="expression" dxfId="2" priority="6">
+  <conditionalFormatting sqref="AE22">
+    <cfRule type="expression" dxfId="31" priority="20">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL8 AT8:AU8 AL9:AU60">
+  <conditionalFormatting sqref="AE22">
+    <cfRule type="expression" dxfId="29" priority="21">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC21">
+    <cfRule type="expression" dxfId="27" priority="8">
+      <formula>PercentComplete</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC21">
+    <cfRule type="expression" dxfId="25" priority="9">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC21">
+    <cfRule type="expression" dxfId="23" priority="10">
+      <formula>Actual</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC21">
+    <cfRule type="expression" dxfId="21" priority="11">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC21">
+    <cfRule type="expression" dxfId="19" priority="12">
+      <formula>Plan</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC21">
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC21">
+    <cfRule type="expression" dxfId="15" priority="14">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15">
+    <cfRule type="expression" dxfId="13" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15">
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15">
+    <cfRule type="expression" dxfId="9" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15">
+    <cfRule type="expression" dxfId="7" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15">
     <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM32:AO32 AP33:AU33 AL33">
-    <cfRule type="expression" dxfId="0" priority="8">
-      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8040,12 +8622,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="9.86328125" customWidth="1"/>
+    <col min="1" max="10" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I6" s="1"/>
     </row>
   </sheetData>

</xml_diff>